<commit_message>
Add content to documentation and results
</commit_message>
<xml_diff>
--- a/Documentation/wyniki.xlsx
+++ b/Documentation/wyniki.xlsx
@@ -12,12 +12,45 @@
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Zdobyslaw</author>
+  </authors>
+  <commentList>
+    <comment ref="H13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zdobyslaw:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Ruchy:</t>
   </si>
@@ -63,12 +96,15 @@
   <si>
     <t>przyspieszenie [ms]</t>
   </si>
+  <si>
+    <t>średnia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +139,19 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -112,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -214,22 +263,41 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -239,94 +307,21 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -343,42 +338,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -400,12 +406,13 @@
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
+          <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.811597825407736E-2"/>
-          <c:y val="9.4681827214627895E-2"/>
-          <c:w val="0.69030789365882783"/>
-          <c:h val="0.83867404646752652"/>
+          <c:x val="0.13862714011914137"/>
+          <c:y val="8.7503245428582024E-2"/>
+          <c:w val="0.80732821718955572"/>
+          <c:h val="0.73598001110494171"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -413,34 +420,85 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$D$12:$D$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ruch f1c4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
-            <a:ln w="28800">
+            <a:ln w="25400">
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="30000"/>
+                <a:srgbClr val="4F81BD">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                  <a:alpha val="51000"/>
                 </a:srgbClr>
               </a:solidFill>
-              <a:custDash>
-                <a:ds d="635000" sp="635000"/>
-                <a:ds d="635000" sp="635000"/>
-              </a:custDash>
+              <a:prstDash val="sysDash"/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="7"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.6137577618349376E-3"/>
+                  <c:y val="-1.1776269426208208E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.6137577618349376E-3"/>
+                  <c:y val="-3.5328808278624682E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1022929603058229E-2"/>
+                  <c:y val="-3.5328808278624682E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1022929603058229E-2"/>
+                  <c:y val="-2.7477961994485864E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3227515523669875E-2"/>
+                  <c:y val="-5.1030500846902319E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.6137577618349376E-3"/>
+                  <c:y val="-3.5328808278624682E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$C$13:$C$18</c:f>
@@ -470,38 +528,38 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz1!$D$13:$D$18</c:f>
+              <c:f>Arkusz1!$H$13:$H$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1041</c:v>
+                  <c:v>1245.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>677</c:v>
+                  <c:v>792</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>463</c:v>
+                  <c:v>613.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>420</c:v>
+                  <c:v>513.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>439</c:v>
+                  <c:v>551.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>464</c:v>
+                  <c:v>584</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="51877760"/>
-        <c:axId val="51876224"/>
+        <c:axId val="86943232"/>
+        <c:axId val="93094656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51876224"/>
+        <c:axId val="93094656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,6 +573,36 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>czas</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t> wyboru ruchu [ms]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6160309155853637E-2"/>
+              <c:y val="0.25622596837407119"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -535,17 +623,40 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51877760"/>
+        <c:crossAx val="86943232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51877760"/>
+        <c:axId val="86943232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>liczba</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t> procesów</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -566,7 +677,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51876224"/>
+        <c:crossAx val="93094656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -580,26 +691,6 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1000" b="0"/>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:spPr>
@@ -609,7 +700,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -626,9 +717,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12099045275424822"/>
-          <c:y val="8.7503238941328887E-2"/>
-          <c:w val="0.64639344498490559"/>
+          <c:x val="0.13127860521038706"/>
+          <c:y val="8.7503107133979616E-2"/>
+          <c:w val="0.6463934449849057"/>
           <c:h val="0.73598001110494171"/>
         </c:manualLayout>
       </c:layout>
@@ -967,11 +1058,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="51991680"/>
-        <c:axId val="51989888"/>
+        <c:axId val="124955264"/>
+        <c:axId val="124952960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51989888"/>
+        <c:axId val="124952960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -995,14 +1086,14 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1050"/>
+                  <a:rPr lang="pl-PL" sz="1200"/>
                   <a:t>czas</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1050" baseline="0"/>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
                   <a:t> wyboru ruchu [ms]</a:t>
                 </a:r>
-                <a:endParaRPr lang="pl-PL" sz="1050"/>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1010,8 +1101,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.8364850876620233E-2"/>
-              <c:y val="0.25622584909497659"/>
+              <c:x val="1.8364850876620237E-2"/>
+              <c:y val="0.25622584909497664"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
@@ -1035,12 +1126,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51991680"/>
+        <c:crossAx val="124955264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51991680"/>
+        <c:axId val="124955264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,18 +1147,25 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
+                  <a:rPr lang="pl-PL" sz="1200"/>
                   <a:t>liczba</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
                   <a:t> procesów</a:t>
                 </a:r>
-                <a:endParaRPr lang="pl-PL"/>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.35675874825891896"/>
+              <c:y val="0.90258965493864818"/>
+            </c:manualLayout>
+          </c:layout>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1089,7 +1187,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51989888"/>
+        <c:crossAx val="124952960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1109,10 +1207,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.80018726829064224"/>
-          <c:y val="0.30738910481831083"/>
+          <c:x val="0.80018726829064213"/>
+          <c:y val="0.30738910481831089"/>
           <c:w val="0.17335770066201805"/>
-          <c:h val="0.28336479733481401"/>
+          <c:h val="0.28336479733481418"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1141,7 +1239,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1158,8 +1256,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12099045275424822"/>
-          <c:y val="8.7503238941328859E-2"/>
+          <c:x val="0.13333622804682499"/>
+          <c:y val="8.7503107133979616E-2"/>
           <c:w val="0.6463934449849057"/>
           <c:h val="0.73598001110494171"/>
         </c:manualLayout>
@@ -1499,11 +1597,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="52005888"/>
-        <c:axId val="51363200"/>
+        <c:axId val="125004416"/>
+        <c:axId val="125002496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51363200"/>
+        <c:axId val="125002496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1527,14 +1625,14 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1050"/>
-                  <a:t>czas</a:t>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>przyspieszenie</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1050" baseline="0"/>
-                  <a:t> wyboru ruchu [ms]</a:t>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t> wyboru ruchu</a:t>
                 </a:r>
-                <a:endParaRPr lang="pl-PL" sz="1050"/>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1542,8 +1640,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.836485087662024E-2"/>
-              <c:y val="0.2562258490949767"/>
+              <c:x val="1.2191982367306411E-2"/>
+              <c:y val="0.25622584909497659"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
@@ -1567,12 +1665,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52005888"/>
+        <c:crossAx val="125004416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52005888"/>
+        <c:axId val="125004416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1588,14 +1686,14 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
+                  <a:rPr lang="pl-PL" sz="1200"/>
                   <a:t>liczba</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
                   <a:t> procesów</a:t>
                 </a:r>
-                <a:endParaRPr lang="pl-PL"/>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1621,7 +1719,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51363200"/>
+        <c:crossAx val="125002496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1641,10 +1739,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.80018726829064202"/>
-          <c:y val="0.30738910481831094"/>
+          <c:x val="0.79401445617757516"/>
+          <c:y val="0.40424688721668589"/>
           <c:w val="0.17335770066201805"/>
-          <c:h val="0.28336479733481434"/>
+          <c:h val="0.28336479733481451"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1673,7 +1771,310 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1342179682779181"/>
+          <c:y val="8.7503245428582024E-2"/>
+          <c:w val="0.80732821718955594"/>
+          <c:h val="0.73598001110494171"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4F81BD">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                  <a:alpha val="51000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.0546749459572664E-2"/>
+                  <c:y val="-3.5328808278624682E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.6137577618349375E-2"/>
+                  <c:y val="-3.5328808278624682E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.0546749459572664E-2"/>
+                  <c:y val="-3.1403385136555238E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.3932991697737737E-2"/>
+                  <c:y val="-4.31796545627635E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1022929603058229E-2"/>
+                  <c:y val="-3.9254231420694091E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.6137577618349402E-3"/>
+                  <c:y val="-3.5328808278624682E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$M$27:$M$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$R$27:$R$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5751491918433933</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0573537454903112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4340759442947553</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2776259635056739</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.142514884306213</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="91212800"/>
+        <c:axId val="91188608"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="91188608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B3B3B3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t>przyspieszenie  wyboru ruchu</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="7.3419654734070521E-3"/>
+              <c:y val="0.18164292867475243"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91212800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="91212800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>liczba</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t> procesów</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91188608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="B3B3B3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1683,10 +2084,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>458550</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>563325</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>79650</xdr:rowOff>
+      <xdr:rowOff>22500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5760719" cy="3235320"/>
     <xdr:graphicFrame macro="">
@@ -1709,9 +2110,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1000154</xdr:colOff>
+      <xdr:colOff>962054</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6172171" cy="3540240"/>
     <xdr:graphicFrame macro="">
@@ -1733,10 +2134,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6172171" cy="3540240"/>
     <xdr:graphicFrame macro="">
@@ -1751,6 +2152,31 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5760719" cy="3235320"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2044,10 +2470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:Q32"/>
+  <dimension ref="C4:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2056,9 +2482,12 @@
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="10" width="10.75" customWidth="1"/>
     <col min="13" max="13" width="15.75" customWidth="1"/>
+    <col min="14" max="14" width="10.25" customWidth="1"/>
+    <col min="15" max="16" width="9.75" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7">
+    <row r="4" spans="3:8">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -2066,319 +2495,377 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:8">
       <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:8">
       <c r="C6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="3:8">
       <c r="C7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:8">
       <c r="C8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:8">
       <c r="C9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="3:7" ht="15" thickBot="1">
+    <row r="10" spans="3:8" ht="15" thickBot="1">
       <c r="C10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="3:7" ht="15.75" thickBot="1">
-      <c r="D11" s="7" t="s">
+    <row r="11" spans="3:8" ht="15.75" thickBot="1">
+      <c r="C11" s="14"/>
+      <c r="D11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="3:7" ht="15.75" thickBot="1">
+    <row r="12" spans="3:8" ht="15">
       <c r="C12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="H12" s="19" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="3:7">
-      <c r="C13" s="10">
+    <row r="13" spans="3:8">
+      <c r="C13" s="20">
         <v>1</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="1">
         <v>1041</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="1">
         <v>1322</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="1">
         <v>1374</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="1">
         <v>1245</v>
       </c>
+      <c r="H13" s="3">
+        <f>AVERAGE(D13:G13)</f>
+        <v>1245.5</v>
+      </c>
     </row>
-    <row r="14" spans="3:7">
-      <c r="C14" s="1">
+    <row r="14" spans="3:8">
+      <c r="C14" s="20">
         <v>2</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>677</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>840</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>783</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="1">
         <v>868</v>
       </c>
+      <c r="H14" s="3">
+        <f t="shared" ref="H14:H18" si="0">AVERAGE(D14:G14)</f>
+        <v>792</v>
+      </c>
     </row>
-    <row r="15" spans="3:7">
-      <c r="C15" s="1">
+    <row r="15" spans="3:8">
+      <c r="C15" s="20">
         <v>3</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>463</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>731</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>601</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="1">
         <v>660</v>
       </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>613.75</v>
+      </c>
     </row>
-    <row r="16" spans="3:7">
-      <c r="C16" s="1">
+    <row r="16" spans="3:8">
+      <c r="C16" s="20">
         <v>4</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>420</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>516</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>539</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="1">
         <v>580</v>
       </c>
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>513.75</v>
+      </c>
     </row>
-    <row r="17" spans="3:17">
-      <c r="C17" s="1">
+    <row r="17" spans="3:18">
+      <c r="C17" s="20">
         <v>5</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>439</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>540</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>582</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="1">
         <v>645</v>
       </c>
+      <c r="H17" s="3">
+        <f t="shared" si="0"/>
+        <v>551.5</v>
+      </c>
     </row>
-    <row r="18" spans="3:17" ht="15" thickBot="1">
-      <c r="C18" s="4">
+    <row r="18" spans="3:18" ht="15" thickBot="1">
+      <c r="C18" s="21">
         <v>6</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="2">
         <v>464</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="2">
         <v>612</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="2">
         <v>612</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="2">
         <v>648</v>
       </c>
+      <c r="H18" s="4">
+        <f t="shared" si="0"/>
+        <v>584</v>
+      </c>
     </row>
-    <row r="24" spans="3:17" ht="15" thickBot="1"/>
-    <row r="25" spans="3:17" ht="15.75" thickBot="1">
-      <c r="N25" s="7" t="s">
+    <row r="24" spans="3:18" ht="15" thickBot="1"/>
+    <row r="25" spans="3:18" ht="15.75" thickBot="1">
+      <c r="M25" s="14"/>
+      <c r="N25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="9"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="3:17" ht="15.75" thickBot="1">
+    <row r="26" spans="3:18" ht="15">
       <c r="M26" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="N26" s="14" t="s">
+      <c r="N26" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O26" s="14" t="s">
+      <c r="O26" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="P26" s="14" t="s">
+      <c r="P26" s="15" t="s">
         <v>10</v>
       </c>
       <c r="Q26" s="15" t="s">
         <v>11</v>
       </c>
+      <c r="R26" s="16" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="27" spans="3:17">
-      <c r="M27" s="10">
+    <row r="27" spans="3:18">
+      <c r="M27" s="17">
         <v>1</v>
       </c>
-      <c r="N27" s="16">
+      <c r="N27" s="8">
         <f>$D$13/D13</f>
         <v>1</v>
       </c>
-      <c r="O27" s="16">
+      <c r="O27" s="8">
         <f>$E$13/E13</f>
         <v>1</v>
       </c>
-      <c r="P27" s="16">
+      <c r="P27" s="8">
         <f>$F$13/F13</f>
         <v>1</v>
       </c>
-      <c r="Q27" s="16">
+      <c r="Q27" s="8">
         <f>$G$13/G13</f>
         <v>1</v>
       </c>
+      <c r="R27" s="9">
+        <f>AVERAGE(N27:Q27)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="3:17">
-      <c r="M28" s="1">
+    <row r="28" spans="3:18">
+      <c r="M28" s="17">
         <v>2</v>
       </c>
-      <c r="N28" s="16">
-        <f t="shared" ref="N28:N32" si="0">$D$13/D14</f>
+      <c r="N28" s="8">
+        <f t="shared" ref="N28:N32" si="1">$D$13/D14</f>
         <v>1.5376661742983753</v>
       </c>
-      <c r="O28" s="16">
-        <f t="shared" ref="O28:O32" si="1">$E$13/E14</f>
+      <c r="O28" s="8">
+        <f t="shared" ref="O28:O32" si="2">$E$13/E14</f>
         <v>1.5738095238095238</v>
       </c>
-      <c r="P28" s="16">
-        <f t="shared" ref="P28:P32" si="2">$F$13/F14</f>
+      <c r="P28" s="8">
+        <f t="shared" ref="P28:P32" si="3">$F$13/F14</f>
         <v>1.7547892720306513</v>
       </c>
-      <c r="Q28" s="16">
-        <f t="shared" ref="Q28:Q32" si="3">$G$13/G14</f>
+      <c r="Q28" s="8">
+        <f t="shared" ref="Q28:Q32" si="4">$G$13/G14</f>
         <v>1.4343317972350231</v>
       </c>
+      <c r="R28" s="9">
+        <f t="shared" ref="R28:R32" si="5">AVERAGE(N28:Q28)</f>
+        <v>1.5751491918433933</v>
+      </c>
     </row>
-    <row r="29" spans="3:17">
-      <c r="M29" s="1">
+    <row r="29" spans="3:18">
+      <c r="M29" s="17">
         <v>3</v>
       </c>
-      <c r="N29" s="16">
-        <f t="shared" si="0"/>
+      <c r="N29" s="8">
+        <f t="shared" si="1"/>
         <v>2.2483801295896328</v>
       </c>
-      <c r="O29" s="16">
+      <c r="O29" s="8">
+        <f t="shared" si="2"/>
+        <v>1.8084815321477428</v>
+      </c>
+      <c r="P29" s="8">
+        <f t="shared" si="3"/>
+        <v>2.2861896838602331</v>
+      </c>
+      <c r="Q29" s="8">
+        <f t="shared" si="4"/>
+        <v>1.8863636363636365</v>
+      </c>
+      <c r="R29" s="9">
+        <f t="shared" si="5"/>
+        <v>2.0573537454903112</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18">
+      <c r="M30" s="17">
+        <v>4</v>
+      </c>
+      <c r="N30" s="8">
         <f t="shared" si="1"/>
-        <v>1.8084815321477428</v>
-      </c>
-      <c r="P29" s="16">
+        <v>2.4785714285714286</v>
+      </c>
+      <c r="O30" s="8">
         <f t="shared" si="2"/>
-        <v>2.2861896838602331</v>
-      </c>
-      <c r="Q29" s="16">
+        <v>2.5620155038759691</v>
+      </c>
+      <c r="P30" s="8">
         <f t="shared" si="3"/>
-        <v>1.8863636363636365</v>
+        <v>2.5491651205936918</v>
+      </c>
+      <c r="Q30" s="8">
+        <f t="shared" si="4"/>
+        <v>2.146551724137931</v>
+      </c>
+      <c r="R30" s="9">
+        <f t="shared" si="5"/>
+        <v>2.4340759442947553</v>
       </c>
     </row>
-    <row r="30" spans="3:17">
-      <c r="M30" s="1">
-        <v>4</v>
-      </c>
-      <c r="N30" s="16">
-        <f t="shared" si="0"/>
-        <v>2.4785714285714286</v>
-      </c>
-      <c r="O30" s="16">
+    <row r="31" spans="3:18">
+      <c r="M31" s="17">
+        <v>5</v>
+      </c>
+      <c r="N31" s="8">
         <f t="shared" si="1"/>
-        <v>2.5620155038759691</v>
-      </c>
-      <c r="P30" s="16">
+        <v>2.3712984054669706</v>
+      </c>
+      <c r="O31" s="8">
         <f t="shared" si="2"/>
-        <v>2.5491651205936918</v>
-      </c>
-      <c r="Q30" s="16">
+        <v>2.4481481481481482</v>
+      </c>
+      <c r="P31" s="8">
         <f t="shared" si="3"/>
-        <v>2.146551724137931</v>
+        <v>2.3608247422680413</v>
+      </c>
+      <c r="Q31" s="8">
+        <f t="shared" si="4"/>
+        <v>1.930232558139535</v>
+      </c>
+      <c r="R31" s="9">
+        <f t="shared" si="5"/>
+        <v>2.2776259635056739</v>
       </c>
     </row>
-    <row r="31" spans="3:17">
-      <c r="M31" s="1">
-        <v>5</v>
-      </c>
-      <c r="N31" s="16">
-        <f t="shared" si="0"/>
-        <v>2.3712984054669706</v>
-      </c>
-      <c r="O31" s="16">
+    <row r="32" spans="3:18" ht="15" thickBot="1">
+      <c r="M32" s="18">
+        <v>6</v>
+      </c>
+      <c r="N32" s="10">
         <f t="shared" si="1"/>
-        <v>2.4481481481481482</v>
-      </c>
-      <c r="P31" s="16">
+        <v>2.2435344827586206</v>
+      </c>
+      <c r="O32" s="10">
         <f t="shared" si="2"/>
-        <v>2.3608247422680413</v>
-      </c>
-      <c r="Q31" s="16">
+        <v>2.1601307189542482</v>
+      </c>
+      <c r="P32" s="10">
         <f t="shared" si="3"/>
-        <v>1.930232558139535</v>
-      </c>
-    </row>
-    <row r="32" spans="3:17" ht="15" thickBot="1">
-      <c r="M32" s="4">
-        <v>6</v>
-      </c>
-      <c r="N32" s="16">
-        <f t="shared" si="0"/>
-        <v>2.2435344827586206</v>
-      </c>
-      <c r="O32" s="16">
-        <f t="shared" si="1"/>
-        <v>2.1601307189542482</v>
-      </c>
-      <c r="P32" s="16">
-        <f t="shared" si="2"/>
         <v>2.2450980392156863</v>
       </c>
-      <c r="Q32" s="16">
-        <f t="shared" si="3"/>
+      <c r="Q32" s="10">
+        <f t="shared" si="4"/>
         <v>1.9212962962962963</v>
+      </c>
+      <c r="R32" s="11">
+        <f t="shared" si="5"/>
+        <v>2.142514884306213</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="N25:R25"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2387,6 +2874,7 @@
     <oddFooter>&amp;CStrona &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>